<commit_message>
Refactoring to AAA, enum constructor, test plan, automation steps, placholder
</commit_message>
<xml_diff>
--- a/class_notes/XYZ-678.xlsx
+++ b/class_notes/XYZ-678.xlsx
@@ -5,15 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdnas/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdnas/eclipse-workspace/NorthEastAAA/class_notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5402549D-8E23-A843-AA09-747279D7C03A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F2574B-48E3-A04B-AF04-790C02E9A7FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="1640" windowWidth="28040" windowHeight="17440" xr2:uid="{6CCF1790-0681-2F4C-B531-C6B6D9F70622}"/>
+    <workbookView xWindow="1100" yWindow="900" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{6CCF1790-0681-2F4C-B531-C6B6D9F70622}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sample Test Plan" sheetId="1" r:id="rId1"/>
+    <sheet name="Test Plan" sheetId="2" r:id="rId2"/>
+    <sheet name="Automation Steps" sheetId="4" r:id="rId3"/>
+    <sheet name="AAA Requirement" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="99">
   <si>
     <t>Test No</t>
   </si>
@@ -181,13 +184,199 @@
   <si>
     <t>3. Open in same tab itself
 4. Same as expected</t>
+  </si>
+  <si>
+    <t>Requirement:</t>
+  </si>
+  <si>
+    <t>1. There will be a pop up to get the zipcode</t>
+  </si>
+  <si>
+    <t>1a. Title will be 'Welcome to Northeast AAA'</t>
+  </si>
+  <si>
+    <t>1b. Sub-Title will be</t>
+  </si>
+  <si>
+    <t>To ensure you receive the best service possible,
+please enter your zip code below:'</t>
+  </si>
+  <si>
+    <t>1c. Footer will be</t>
+  </si>
+  <si>
+    <t>AAA Northeast serves members in CT, MA, NH, NJ, NY &amp; RI.'</t>
+  </si>
+  <si>
+    <t>3. there will be a button 'Submit'</t>
+  </si>
+  <si>
+    <t>3a. Upon clicking on submit, user will land into homepage of AAA</t>
+  </si>
+  <si>
+    <t>Footer</t>
+  </si>
+  <si>
+    <t>Zipcode field</t>
+  </si>
+  <si>
+    <t>Submit button</t>
+  </si>
+  <si>
+    <t>Sub - title</t>
+  </si>
+  <si>
+    <t>Verify Title</t>
+  </si>
+  <si>
+    <t>Verify sub-title</t>
+  </si>
+  <si>
+    <t>Verify Footer</t>
+  </si>
+  <si>
+    <t>Verify Zipcode field</t>
+  </si>
+  <si>
+    <t>Verify submit button</t>
+  </si>
+  <si>
+    <t>Pre-Steps/Conditions</t>
+  </si>
+  <si>
+    <t>Navigate to &lt;url&gt;</t>
+  </si>
+  <si>
+    <t>1. Verify the sub-title 'To ensure you receive the best service possible,
+please enter your zip code below:'</t>
+  </si>
+  <si>
+    <t>1. Sub-title will be visible and 'To ensure you receive the best service possible,
+please enter your zip code below:'</t>
+  </si>
+  <si>
+    <t>1. Verify footer 'AAA Northeast serves members in CT, MA, NH, NJ, NY &amp; RI.'</t>
+  </si>
+  <si>
+    <t>1. Footer will be visible and 'AAA Northeast serves members in CT, MA, NH, NJ, NY &amp; RI.'</t>
+  </si>
+  <si>
+    <t>1. Verify there is a pop-up
+2. Verify the title 'Welcome to Northeast AAA'</t>
+  </si>
+  <si>
+    <t>1. Pop-up will appears when user naviagte into AAA
+2. Title will be visble and 'Welcome to Northeast AAA'</t>
+  </si>
+  <si>
+    <t>Pop-up and Title</t>
+  </si>
+  <si>
+    <t>3b. If zipcode is empty,upon clicking submit button error in red will appears 'zipcode is required'</t>
+  </si>
+  <si>
+    <t>1. Click submit button without inserting 'zipcode'
+2. Insert a valid zipcode
+3. Click submit button
+4. Verify AAA homepage title</t>
+  </si>
+  <si>
+    <t>1. An error message will pop up in red color and 'Zipcode is required'
+4a. Pop up will disappears
+4b. Title of the homepage will be 'Northeast AAA'</t>
+  </si>
+  <si>
+    <t>2. zipcode filed will take any input and it will be in the middle. Length is limited to 5 character</t>
+  </si>
+  <si>
+    <t>XYZ-234</t>
+  </si>
+  <si>
+    <t>1. Error message is in black and the error message is 'Please enter a valid ZIP code so we can direct you to the
+AAA website in your area.'
+4a. Same as expected
+4b. Same as expected</t>
+  </si>
+  <si>
+    <t>1. Verify zipcode field in the middle
+2. Input numbers
+3. Input words
+4. Input alpahnumeric
+5. input length will be 5</t>
+  </si>
+  <si>
+    <t>1. Zipcode field will be in the middle
+2. Zipcode will take numbers as input
+3. Zipcode will take words as inputs
+4. Zipcode will take alphanumeric as input
+5. Input length will be 5</t>
+  </si>
+  <si>
+    <t>Same as expected</t>
+  </si>
+  <si>
+    <t>Validation</t>
+  </si>
+  <si>
+    <t>Actions</t>
+  </si>
+  <si>
+    <t>assertEqual(expected, actual)</t>
+  </si>
+  <si>
+    <t>Assert</t>
+  </si>
+  <si>
+    <t>Zipcode - words</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Zipcode - numbers</t>
+  </si>
+  <si>
+    <t>Zipcode - alphanumeric</t>
+  </si>
+  <si>
+    <t>verify length</t>
+  </si>
+  <si>
+    <t>getAttributes("maxlength")</t>
+  </si>
+  <si>
+    <t>clear()</t>
+  </si>
+  <si>
+    <t>Sumbit button</t>
+  </si>
+  <si>
+    <t>Click()</t>
+  </si>
+  <si>
+    <t>Verify error messsage</t>
+  </si>
+  <si>
+    <t>get max length</t>
+  </si>
+  <si>
+    <t>Step no</t>
+  </si>
+  <si>
+    <t>clean-up the field</t>
+  </si>
+  <si>
+    <t>Verify Homepage Title</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -223,8 +412,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -243,8 +454,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -424,11 +647,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -456,9 +690,21 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -775,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D040B64-FD02-9843-9106-9D6FBDBB23D6}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1087,4 +1333,757 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAE362DE-00A4-274D-B396-D4AF86DFC7E3}">
+  <dimension ref="A1:M6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="12"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="16"/>
+      <c r="M2" s="13"/>
+    </row>
+    <row r="3" spans="1:13" ht="85" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" s="12"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="16"/>
+      <c r="M3" s="13"/>
+    </row>
+    <row r="4" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="I4" s="12"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="16"/>
+      <c r="M4" s="17"/>
+    </row>
+    <row r="5" spans="1:13" ht="153" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="J5" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5" s="17"/>
+    </row>
+    <row r="6" spans="1:13" ht="154" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="I6" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="J6" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71F95DB3-AE73-E845-B4D6-7E8761BEE1F5}">
+  <dimension ref="A1:F34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" customWidth="1"/>
+    <col min="3" max="3" width="36.83203125" customWidth="1"/>
+    <col min="4" max="4" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1.01</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2">
+        <v>1.7</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2">
+        <v>1.9</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F339E64-B71F-9341-A1C3-87E6AE3E418A}">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="105.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Reporter.log, index.html, getAttribute, RTM, clear
</commit_message>
<xml_diff>
--- a/class_notes/XYZ-678.xlsx
+++ b/class_notes/XYZ-678.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdnas/eclipse-workspace/NorthEastAAA/class_notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F2574B-48E3-A04B-AF04-790C02E9A7FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A6C577-DE80-4F47-B63C-A7B86D0C5DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="900" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{6CCF1790-0681-2F4C-B531-C6B6D9F70622}"/>
+    <workbookView xWindow="1100" yWindow="900" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{6CCF1790-0681-2F4C-B531-C6B6D9F70622}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample Test Plan" sheetId="1" r:id="rId1"/>
     <sheet name="Test Plan" sheetId="2" r:id="rId2"/>
     <sheet name="Automation Steps" sheetId="4" r:id="rId3"/>
     <sheet name="AAA Requirement" sheetId="3" r:id="rId4"/>
+    <sheet name="RTM" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="123">
   <si>
     <t>Test No</t>
   </si>
@@ -192,9 +193,6 @@
     <t>1. There will be a pop up to get the zipcode</t>
   </si>
   <si>
-    <t>1a. Title will be 'Welcome to Northeast AAA'</t>
-  </si>
-  <si>
     <t>1b. Sub-Title will be</t>
   </si>
   <si>
@@ -263,10 +261,6 @@
   <si>
     <t>1. Verify there is a pop-up
 2. Verify the title 'Welcome to Northeast AAA'</t>
-  </si>
-  <si>
-    <t>1. Pop-up will appears when user naviagte into AAA
-2. Title will be visble and 'Welcome to Northeast AAA'</t>
   </si>
   <si>
     <t>Pop-up and Title</t>
@@ -371,12 +365,92 @@
   <si>
     <t>Done</t>
   </si>
+  <si>
+    <t>1. Same as expected
+2. Title is 'Welcome to AAA Northeast'</t>
+  </si>
+  <si>
+    <t>1. Same as expected</t>
+  </si>
+  <si>
+    <t>1. Pop-up will appears when user naviagte into AAA
+2. Title will be visble and 'Welcome to AAA Northeast'</t>
+  </si>
+  <si>
+    <t>1a. Title will be 'Welcome to AAA Northeast'</t>
+  </si>
+  <si>
+    <t>User Req No</t>
+  </si>
+  <si>
+    <t>Sys Req No</t>
+  </si>
+  <si>
+    <t>Test Case No</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Ticket</t>
+  </si>
+  <si>
+    <t>XYZ-678</t>
+  </si>
+  <si>
+    <t>3.1.6</t>
+  </si>
+  <si>
+    <t>3.1.7</t>
+  </si>
+  <si>
+    <t>3.1.8</t>
+  </si>
+  <si>
+    <t>2.0.f.5</t>
+  </si>
+  <si>
+    <t>2.0.f.6</t>
+  </si>
+  <si>
+    <t>2.0.f.7</t>
+  </si>
+  <si>
+    <t>TC_XYZ-678_1</t>
+  </si>
+  <si>
+    <t>TC_XYZ-678_2</t>
+  </si>
+  <si>
+    <t>TC_XYZ-678_3</t>
+  </si>
+  <si>
+    <t>TC_XYZ-678_4</t>
+  </si>
+  <si>
+    <t>TC_XYZ-678_5</t>
+  </si>
+  <si>
+    <t>XYZ-234 Defect has been created</t>
+  </si>
+  <si>
+    <t>Test Status</t>
+  </si>
+  <si>
+    <t>Automate</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Automation not required</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -434,8 +508,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -466,6 +547,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -662,7 +749,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -699,12 +786,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1340,12 +1428,12 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
@@ -1377,7 +1465,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>3</v>
@@ -1402,11 +1490,11 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="68" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
-        <v>1</v>
+      <c r="A2" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>27</v>
@@ -1415,19 +1503,23 @@
         <v>28</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="I2" s="12"/>
-      <c r="J2" s="13"/>
+        <v>99</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="J2" s="24" t="s">
+        <v>36</v>
+      </c>
       <c r="K2" s="11" t="s">
         <v>14</v>
       </c>
@@ -1435,11 +1527,11 @@
       <c r="M2" s="13"/>
     </row>
     <row r="3" spans="1:13" ht="85" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
-        <v>2</v>
+      <c r="A3" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>29</v>
@@ -1448,19 +1540,23 @@
         <v>32</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F3" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="H3" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="I3" s="12"/>
-      <c r="J3" s="13"/>
+      <c r="I3" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="J3" s="24" t="s">
+        <v>36</v>
+      </c>
       <c r="K3" s="11" t="s">
         <v>14</v>
       </c>
@@ -1468,11 +1564,11 @@
       <c r="M3" s="13"/>
     </row>
     <row r="4" spans="1:13" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <v>3</v>
+      <c r="A4" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>30</v>
@@ -1481,19 +1577,23 @@
         <v>33</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G4" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="H4" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="I4" s="12"/>
-      <c r="J4" s="19"/>
+      <c r="I4" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="J4" s="24" t="s">
+        <v>36</v>
+      </c>
       <c r="K4" s="11" t="s">
         <v>14</v>
       </c>
@@ -1501,11 +1601,11 @@
       <c r="M4" s="17"/>
     </row>
     <row r="5" spans="1:13" ht="153" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <v>4</v>
+      <c r="A5" s="2" t="s">
+        <v>116</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>30</v>
@@ -1514,19 +1614,19 @@
         <v>33</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G5" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="I5" s="12" t="s">
         <v>77</v>
-      </c>
-      <c r="H5" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>79</v>
       </c>
       <c r="J5" s="24" t="s">
         <v>36</v>
@@ -1540,11 +1640,11 @@
       <c r="M5" s="17"/>
     </row>
     <row r="6" spans="1:13" ht="154" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>5</v>
+      <c r="A6" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>31</v>
@@ -1553,19 +1653,19 @@
         <v>34</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I6" s="22" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J6" s="23" t="s">
         <v>41</v>
@@ -1577,10 +1677,11 @@
         <v>15</v>
       </c>
       <c r="M6" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1589,8 +1690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71F95DB3-AE73-E845-B4D6-7E8761BEE1F5}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1607,16 +1708,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C1" s="25" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F1" s="25" t="s">
         <v>6</v>
@@ -1630,16 +1731,16 @@
         <v>1.01</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1648,16 +1749,16 @@
         <v>1.2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1666,16 +1767,16 @@
         <v>1.3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1684,14 +1785,14 @@
         <v>1.4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1700,16 +1801,16 @@
         <v>1.5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1718,14 +1819,14 @@
         <v>1.6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1734,13 +1835,13 @@
         <v>1.7</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1749,16 +1850,16 @@
         <v>1.8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1767,13 +1868,15 @@
         <v>1.9</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
@@ -1781,13 +1884,15 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
@@ -1795,15 +1900,17 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F12" s="2"/>
+        <v>80</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
@@ -1811,13 +1918,15 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
@@ -1825,13 +1934,15 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="F14" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
@@ -1839,15 +1950,17 @@
         <v>1.1399999999999999</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F15" s="2"/>
+        <v>80</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
@@ -1855,13 +1968,15 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="F16" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
@@ -1869,15 +1984,17 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F17" s="2"/>
+        <v>80</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
@@ -2021,7 +2138,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F339E64-B71F-9341-A1C3-87E6AE3E418A}">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2040,50 +2159,236 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B17E00D2-3492-6B4D-8B9A-97D75162BDE7}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>